<commit_message>
Edited TimeStamp ftom 10 to 12 in HomeWork3.xlsx
</commit_message>
<xml_diff>
--- a/HomeWork3.xlsx
+++ b/HomeWork3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ученики и классы" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,6 +34,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Кабинеты могут иметь и буквенно цифровые обозначения</t>
         </r>
@@ -548,11 +549,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -573,14 +575,10 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -595,6 +593,7 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -716,6 +715,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -732,14 +735,14 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -748,10 +751,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -788,7 +787,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -883,17 +882,17 @@
       <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.14"/>
   </cols>
@@ -1509,7 +1508,7 @@
         <v>98</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1546,55 +1545,55 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="10" t="s">
         <v>106</v>
       </c>
       <c r="J29" s="7"/>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L29" s="10" t="n">
+      <c r="L29" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="M29" s="11" t="s">
+      <c r="M29" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="10" t="n">
+      <c r="E30" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="14" t="s">
         <v>111</v>
       </c>
       <c r="J30" s="7"/>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="L30" s="10" t="n">
+      <c r="L30" s="11" t="n">
         <v>4</v>
       </c>
       <c r="M30" s="7" t="s">
@@ -1602,64 +1601,64 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="10" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="10" t="n">
+      <c r="E32" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="10" t="n">
+      <c r="E33" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="10" t="n">
+      <c r="E34" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="13" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1684,18 +1683,18 @@
   </sheetPr>
   <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="12.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="17" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.16"/>
   </cols>
@@ -1751,16 +1750,16 @@
         <v>129</v>
       </c>
       <c r="G4" s="0"/>
-      <c r="H4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="10" t="n">
+      <c r="H4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1778,16 +1777,16 @@
         <v>130</v>
       </c>
       <c r="G5" s="0"/>
-      <c r="H5" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="n">
+      <c r="H5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1805,16 +1804,16 @@
         <v>131</v>
       </c>
       <c r="G6" s="0"/>
-      <c r="H6" s="10" t="n">
+      <c r="H6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" s="10" t="n">
+      <c r="I6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1832,16 +1831,16 @@
         <v>132</v>
       </c>
       <c r="G7" s="0"/>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="10" t="n">
+      <c r="I7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1859,16 +1858,16 @@
         <v>133</v>
       </c>
       <c r="G8" s="0"/>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="10" t="n">
+      <c r="I8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="K8" s="10" t="n">
+      <c r="K8" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1886,16 +1885,16 @@
         <v>134</v>
       </c>
       <c r="G9" s="0"/>
-      <c r="H9" s="10" t="n">
+      <c r="H9" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="I9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10" t="n">
+      <c r="I9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="10" t="n">
+      <c r="K9" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1913,16 +1912,16 @@
         <v>135</v>
       </c>
       <c r="G10" s="0"/>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="I10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="10" t="n">
+      <c r="I10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="10" t="n">
+      <c r="K10" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1940,16 +1939,16 @@
         <v>136</v>
       </c>
       <c r="G11" s="0"/>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="10" t="n">
+      <c r="I11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="K11" s="10" t="n">
+      <c r="K11" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1967,16 +1966,16 @@
         <v>137</v>
       </c>
       <c r="G12" s="0"/>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="I12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="10" t="n">
+      <c r="I12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="K12" s="10" t="n">
+      <c r="K12" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1994,16 +1993,16 @@
         <v>138</v>
       </c>
       <c r="G13" s="0"/>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="I13" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10" t="n">
+      <c r="I13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="K13" s="10" t="n">
+      <c r="K13" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2021,16 +2020,16 @@
         <v>139</v>
       </c>
       <c r="G14" s="0"/>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="I14" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10" t="n">
+      <c r="I14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="K14" s="10" t="n">
+      <c r="K14" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2048,64 +2047,64 @@
         <v>140</v>
       </c>
       <c r="G15" s="0"/>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="I15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="10" t="n">
+      <c r="I15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="K15" s="10" t="n">
+      <c r="K15" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G16" s="0"/>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="I16" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="10" t="n">
+      <c r="I16" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="0"/>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="I17" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J17" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="10" t="n">
+      <c r="I17" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>120</v>
       </c>
       <c r="G18" s="0"/>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="I18" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J18" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K18" s="10" t="n">
+      <c r="I18" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2126,128 +2125,128 @@
         <v>9</v>
       </c>
       <c r="G19" s="0"/>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="I19" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J19" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K19" s="10" t="n">
+      <c r="I19" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="10" t="n">
+      <c r="E20" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>142</v>
       </c>
       <c r="G20" s="0"/>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="I20" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J20" s="10" t="n">
+      <c r="I20" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="K20" s="10" t="n">
+      <c r="K20" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E21" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>145</v>
       </c>
       <c r="G21" s="0"/>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="I21" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J21" s="10" t="n">
+      <c r="I21" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="K21" s="10" t="n">
+      <c r="K21" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>109</v>
       </c>
       <c r="E22" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="15" t="s">
         <v>147</v>
       </c>
       <c r="G22" s="0"/>
-      <c r="H22" s="10" t="n">
+      <c r="H22" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="I22" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J22" s="10" t="n">
+      <c r="I22" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="K22" s="10" t="n">
+      <c r="K22" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>118</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="11" t="n">
         <v>100</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>148</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I23" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J23" s="10" t="n">
+      <c r="I23" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="K23" s="10" t="n">
+      <c r="K23" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2258,16 +2257,16 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="0"/>
-      <c r="H24" s="10" t="n">
+      <c r="H24" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="I24" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J24" s="10" t="n">
+      <c r="I24" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="K24" s="10" t="n">
+      <c r="K24" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2278,16 +2277,16 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="0"/>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="I25" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J25" s="10" t="n">
+      <c r="I25" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J25" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="K25" s="10" t="n">
+      <c r="K25" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2298,16 +2297,16 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="0"/>
-      <c r="H26" s="10" t="n">
+      <c r="H26" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="I26" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J26" s="10" t="n">
+      <c r="I26" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="K26" s="10" t="n">
+      <c r="K26" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2318,16 +2317,16 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="0"/>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="I27" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J27" s="10" t="n">
+      <c r="I27" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J27" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="K27" s="10" t="n">
+      <c r="K27" s="11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2360,7 +2359,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="9" t="s">
         <v>121</v>
       </c>
       <c r="I30" s="0"/>
@@ -2392,11 +2391,11 @@
       <c r="H32" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11"/>
+      <c r="J32" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="K32" s="10" t="n">
+      <c r="K32" s="11" t="n">
         <v>10</v>
       </c>
       <c r="L32" s="21" t="s">
@@ -2407,11 +2406,11 @@
       <c r="H33" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10" t="s">
+      <c r="I33" s="11"/>
+      <c r="J33" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="K33" s="10" t="n">
+      <c r="K33" s="11" t="n">
         <v>3</v>
       </c>
       <c r="L33" s="7" t="s">
@@ -2422,11 +2421,11 @@
       <c r="H34" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10" t="s">
+      <c r="I34" s="11"/>
+      <c r="J34" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="K34" s="10" t="n">
+      <c r="K34" s="11" t="n">
         <v>3</v>
       </c>
       <c r="L34" s="7" t="s">
@@ -2437,11 +2436,11 @@
       <c r="H35" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10" t="s">
+      <c r="I35" s="11"/>
+      <c r="J35" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="K35" s="10" t="n">
+      <c r="K35" s="11" t="n">
         <v>3</v>
       </c>
       <c r="L35" s="7" t="s">
@@ -2472,11 +2471,11 @@
   </sheetPr>
   <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="15.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="23" width="11.52"/>
@@ -2508,14 +2507,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="11" t="n">
         <v>10</v>
       </c>
       <c r="F4" s="27" t="s">
@@ -2523,50 +2522,50 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E5" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="E6" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="11" t="n">
         <v>10</v>
       </c>
       <c r="F7" s="21" t="s">
@@ -2574,32 +2573,32 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E9" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>